<commit_message>
WBCAMS-552 [WorkBC.ca] Update SSOT with July Monthly Labour Force Survey data
</commit_message>
<xml_diff>
--- a/migration/data/WorkBC LMS July_2024.xlsx
+++ b/migration/data/WorkBC LMS July_2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CEU\7. WORKBC and PROJECTS\LMI Data Updates\Monthly Labour Force Survey\Drupal\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgreensi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DDA2FCC-51C0-4EBD-BB04-46E3565BEF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F863F8A7-21D0-45AA-BA6C-55ED257D69BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>BC Employment Trends</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>July  2023</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -1193,6 +1196,9 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1213,9 +1219,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="86">
@@ -1728,14 +1731,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBC98A6-26E3-4693-9BA5-07FBC64A5104}">
-  <dimension ref="A1"/>
+  <dimension ref="J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="12" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1745,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
@@ -1765,11 +1774,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="28">
@@ -1802,11 +1811,11 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
       <c r="E6" s="51"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -1938,11 +1947,11 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
       <c r="D15" s="13"/>
       <c r="E15" s="1"/>
       <c r="I15" s="16"/>
@@ -2112,10 +2121,10 @@
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="57"/>
+      <c r="B25" s="58"/>
       <c r="E25" s="1"/>
       <c r="J25" s="16"/>
       <c r="K25" s="20"/>
@@ -2267,11 +2276,11 @@
       <c r="L34" s="16"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A35" s="52" t="s">
+      <c r="A35" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="52"/>
-      <c r="C35" s="52"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
       <c r="G35" s="20"/>
       <c r="H35" s="16"/>
       <c r="I35" s="20"/>
@@ -2316,11 +2325,11 @@
       <c r="K38" s="4"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A39" s="58" t="s">
+      <c r="A39" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="58"/>
-      <c r="C39" s="58"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
       <c r="D39" s="13"/>
       <c r="E39" s="1"/>
       <c r="H39" s="20"/>
@@ -2619,11 +2628,11 @@
       <c r="L56" s="4"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A57" s="55" t="s">
+      <c r="A57" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
+      <c r="B57" s="56"/>
+      <c r="C57" s="56"/>
       <c r="D57" s="13"/>
       <c r="E57" s="26"/>
       <c r="G57" s="20"/>
@@ -2945,7 +2954,7 @@
       <c r="B73" s="45">
         <v>-2.6</v>
       </c>
-      <c r="C73" s="59">
+      <c r="C73" s="52">
         <v>-2500</v>
       </c>
       <c r="D73" s="4"/>

</xml_diff>